<commit_message>
Created logic for harvester detail.
</commit_message>
<xml_diff>
--- a/Content/Tractors/Tractor_Image_Infos1.xlsx
+++ b/Content/Tractors/Tractor_Image_Infos1.xlsx
@@ -14,96 +14,321 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="108">
+  <si>
+    <t>Powertrac Tractors</t>
+  </si>
+  <si>
+    <t>Sonalika Tractors</t>
+  </si>
+  <si>
+    <t>New Holland Tractors</t>
+  </si>
+  <si>
+    <t>Massey Ferguson Tractors</t>
+  </si>
   <si>
     <t>Mahindra Tractors</t>
   </si>
   <si>
+    <t>Kubota Tractors</t>
+  </si>
+  <si>
+    <t>Farmtrac Tractors</t>
+  </si>
+  <si>
+    <t>John Deere Tractors</t>
+  </si>
+  <si>
     <t>Eicher Tractors</t>
   </si>
   <si>
     <t>Swaraj Tractors</t>
   </si>
   <si>
-    <t>Sonalika Tractors</t>
-  </si>
-  <si>
-    <t>Kubota Tractors</t>
-  </si>
-  <si>
-    <t>New Holland Tractors</t>
-  </si>
-  <si>
-    <t>Farmtrac Tractors</t>
-  </si>
-  <si>
-    <t>Powertrac Tractors</t>
-  </si>
-  <si>
-    <t>ARJUN NOVO 605 DI–i-4WD</t>
+    <t>Autonxt Tractors</t>
+  </si>
+  <si>
+    <t>Digitrac Tractors</t>
+  </si>
+  <si>
+    <t>Hindustan Tractors</t>
+  </si>
+  <si>
+    <t>Euro 50</t>
+  </si>
+  <si>
+    <t>745 DI III Sikander</t>
+  </si>
+  <si>
+    <t>3630 Tx Special Edition</t>
+  </si>
+  <si>
+    <t>DI 35</t>
+  </si>
+  <si>
+    <t>1035 DI</t>
+  </si>
+  <si>
+    <t>Yuvo 575 DI 4WD</t>
+  </si>
+  <si>
+    <t>MU4501 2WD</t>
+  </si>
+  <si>
+    <t>45 Powermaxx</t>
+  </si>
+  <si>
+    <t>275 DI TU XP Plus</t>
+  </si>
+  <si>
+    <t>Arjun Novo 605 Di-i 2WD</t>
+  </si>
+  <si>
+    <t>5050 D - 4WD</t>
+  </si>
+  <si>
+    <t>7250 Power Up</t>
+  </si>
+  <si>
+    <t>5045 D 4WD</t>
+  </si>
+  <si>
+    <t>5210</t>
+  </si>
+  <si>
+    <t>242</t>
+  </si>
+  <si>
+    <t>Oja 3140 4WD</t>
+  </si>
+  <si>
+    <t>744 FE 4WD</t>
+  </si>
+  <si>
+    <t>475 DI XP Plus</t>
+  </si>
+  <si>
+    <t>5105</t>
   </si>
   <si>
     <t>380</t>
   </si>
   <si>
+    <t>60 PowerMaxx</t>
+  </si>
+  <si>
     <t>Code</t>
   </si>
   <si>
-    <t>DI 35</t>
-  </si>
-  <si>
-    <t>Arjun Novo 605 Di-i 2WD</t>
-  </si>
-  <si>
-    <t>MU4501 2WD</t>
-  </si>
-  <si>
-    <t>Yuvo 575 DI 4WD</t>
-  </si>
-  <si>
-    <t>3630 Tx Special Edition</t>
-  </si>
-  <si>
-    <t>275 DI TU XP Plus</t>
-  </si>
-  <si>
-    <t>45 Powermaxx</t>
-  </si>
-  <si>
-    <t>Euro 50</t>
-  </si>
-  <si>
-    <t>['img0-mahindra-arjun-novo-605-dii-4wd-1698917936.png', 'img1-mahindra-arjun-novo-605-dii-4wd-16989179360.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+    <t>JIVO 245 DI</t>
+  </si>
+  <si>
+    <t>Euro 439</t>
+  </si>
+  <si>
+    <t>X45H2</t>
+  </si>
+  <si>
+    <t>8055 Magnatrak</t>
+  </si>
+  <si>
+    <t>PP 46i</t>
+  </si>
+  <si>
+    <t>5310</t>
+  </si>
+  <si>
+    <t>475 DI</t>
+  </si>
+  <si>
+    <t>485</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>3032 Nx</t>
+  </si>
+  <si>
+    <t>YUVO TECH Plus 415 DI</t>
+  </si>
+  <si>
+    <t>3230 TX Super</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>Simba 20 4WD</t>
+  </si>
+  <si>
+    <t>3230 NX</t>
+  </si>
+  <si>
+    <t>551 4WD Prima G3</t>
+  </si>
+  <si>
+    <t>6120 B</t>
+  </si>
+  <si>
+    <t>42 DI Sikander</t>
+  </si>
+  <si>
+    <t>Euro 50 Next</t>
+  </si>
+  <si>
+    <t>735 XT</t>
+  </si>
+  <si>
+    <t>3600 Tx Heritage Edition</t>
+  </si>
+  <si>
+    <t>DI 750III</t>
+  </si>
+  <si>
+    <t>Arjun Novo 605 Di-ps</t>
+  </si>
+  <si>
+    <t>735 FE E</t>
+  </si>
+  <si>
+    <t>['img0-euro-50-1632287717.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-745-di-iii-sikander-1631526194.png', 'img1-upload-1631526194-0.png', 'img2-upload-1631526194-0.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-new-holland-3630-tx-special-edition-1689916088.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-new-holland-3630-tx-special-edition-1689916088.png']</t>
+  </si>
+  <si>
+    <t>['img0-di-35-1631526570.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-di-35-1631526570.png']</t>
+  </si>
+  <si>
+    <t>['img0-1035-di-1632210763.png', 'img1-upload-1632210763-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-yuvo-575-di-4wd-1632209384.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-yuvo-575-di-4wd-1632209384.png']</t>
+  </si>
+  <si>
+    <t>['img0-kubota-mu4501-2wd.png', 'img1-upload-1632223345-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-farmtrac-45-powermaxx-1690540103.png', 'img1-farmtrac-45-powermaxx-16905401030.png', 'img2-farmtrac-45-powermaxx-16905401030.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-275-di-tu-xp-plus-1632304804.png', 'img1-275-di-tu-xp-plus-1632304804.png', 'img2-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-arjun-novo-605-di-i-1632207718.png', 'img1-upload-1632207719-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-5050-d-4wd-1632220996.png', 'img1-upload-1632220996-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-7250-power-up-1641816187.png', 'img1-upload-1641816187-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-5045-d-4wd-1632375798.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-5210-1632222316.png', 'img1-5210-1632222316.png']</t>
+  </si>
+  <si>
+    <t>['img0-242-1632219585.png', 'img1-242-1632219585.png', 'img2-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-mahindra-oja-3140-4wd-1692164169.png', 'img1-mahindra-oja-3140-4wd-16921699120.png', 'img2-mahindra-oja-3140-4wd-16921703420.png', 'img3-mahindra-oja-3140-4wd-16921699120.png']</t>
+  </si>
+  <si>
+    <t>['img0-744-fe-4wd-1631014809.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-744-fe-4wd-1631014809.png']</t>
+  </si>
+  <si>
+    <t>['img0-475-di-xp-plus-1632207172.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-5105-1632222132.png', 'img1-upload-1632222132-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
   </si>
   <si>
     <t>['img0-380-1632220220.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
   </si>
   <si>
+    <t>['img0-farmtrac-60-powermaxx-1690541201.png', 'img1-farmtrac-60-powermaxx-16905412010.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
     <t>['img0-code-1646204065.png', 'img1-code-1646204065.png', 'img2-mqdefault.png']</t>
   </si>
   <si>
-    <t>['img0-di-35-1631526570.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-di-35-1631526570.png']</t>
-  </si>
-  <si>
-    <t>['img0-arjun-novo-605-di-i-1632207718.png', 'img1-upload-1632207719-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['img0-kubota-mu4501-2wd.png', 'img1-upload-1632223345-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['img0-yuvo-575-di-4wd-1632209384.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-yuvo-575-di-4wd-1632209384.png']</t>
-  </si>
-  <si>
-    <t>['img0-new-holland-3630-tx-special-edition-1689916088.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-new-holland-3630-tx-special-edition-1689916088.png']</t>
-  </si>
-  <si>
-    <t>['img0-275-di-tu-xp-plus-1632304804.png', 'img1-275-di-tu-xp-plus-1632304804.png', 'img2-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['img0-farmtrac-45-powermaxx-1690540103.png', 'img1-farmtrac-45-powermaxx-16905401030.png', 'img2-farmtrac-45-powermaxx-16905401030.png', 'img3-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['img0-euro-50-1632287717.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+    <t>['img0-jivo-245-di-1632208438.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-euro-439-1632287035.png', 'img1-euro-439-1632287035.png', 'img2-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-autonxt-x45h2.png', 'img1-autonxt-x45h2.png']</t>
+  </si>
+  <si>
+    <t>['img0-8055-magnatrak-1649221137.png', 'img1-upload-1649221137-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-digitrac-pp-46i7.png', 'img1-upload-1647864809-0.png', 'img2-upload-1647864809-0.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-5310-1632222719.png', 'img1-upload-1632222719-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-475-di-1632207012.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-475-di-1632207012.png']</t>
+  </si>
+  <si>
+    <t>['img0-485-1632220359.png', 'img1-485-1632220359.png', 'img2-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-60-1632286457.png', 'img1-upload-1632286457-0.png', 'img2-upload-1632286457-0.png', 'img3-qh304TQ7bzE_sddefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-3032-nx-1636612236.png', 'img1-upload-1636612236-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-yuvo-tech-plus-415-di-1633952706.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-yuvo-tech-plus-415-di-1633952706.png']</t>
+  </si>
+  <si>
+    <t>['img0-3230-tx-super-1632215453.png', 'img1-upload-1632215453-0.png', 'img2-upload-1632215453-0.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-333-1635157048.png', 'img1-upload-1635157048-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-new-holland-simba-20-4wd-1694673653.png', 'img1-new-holland-simba-20-4wd-16946736530.png', 'img2-new-holland-simba-20-4wd-1694673653.png', 'img3-new-holland-simba-20-4wd-16946736530.png']</t>
+  </si>
+  <si>
+    <t>['img0-3230-nx-1632215295.png', 'img1-upload-1632215295-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-massey-ferguson-551-4wd-prima-g3-1695291196.png', 'img1-massey-ferguson-551-4wd-prima-g3-16952911960.png', 'img2-massey-ferguson-551-4wd-prima-g3-1695291196.png', 'img3-massey-ferguson-551-4wd-prima-g3-16952911960.png']</t>
+  </si>
+  <si>
+    <t>['img0-6120-b-1632223212.png', 'img1-6120-b-1632223212.png', 'img2-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-42-di-sikander-1631525877.png', 'img1-upload-1631525877-0.png', 'img2-upload-1631525877-0.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-powertrac-euro-50-next-1690880901.png', 'img1-powertrac-euro-50-next-16908809010.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-735-xt-1631014365.png', 'img1-735-xt-1631014365.png', 'img2-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-3600-tx-heritage-edition-1632216924.png', 'img1-upload-1632216924-0.png', 'img2-3600-tx-heritage-edition-1632216924.png', 'img3-upload-1632216924-0.png']</t>
+  </si>
+  <si>
+    <t>['img0-di-750iii-1631529270.png', 'img1-upload-1631529270-0.png', 'img2-di-750iii-1631529270.png', 'img3-upload-1631529270-0.png']</t>
+  </si>
+  <si>
+    <t>['img0-arjun-novo-605-di-ps-1632208041.png', 'img1-upload-1632208041-0.png', 'img2-upload-1632208041-0.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-swaraj-735-fe-e-1701335706.png', 'img1-swaraj-735-fe-e-17013357060.png', 'img2-swaraj-735-fe-e-1701335706.png', 'img3-swaraj-735-fe-e-17013357060.png']</t>
   </si>
   <si>
     <t>Brand</t>
@@ -468,7 +693,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -476,13 +701,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -490,131 +715,131 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -622,10 +847,10 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -633,21 +858,626 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
         <v>1</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
-        <v>20</v>
+      <c r="B44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" t="s">
+        <v>42</v>
+      </c>
+      <c r="C52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" t="s">
+        <v>49</v>
+      </c>
+      <c r="C57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>50</v>
+      </c>
+      <c r="C58" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>52</v>
+      </c>
+      <c r="C62" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" t="s">
+        <v>40</v>
+      </c>
+      <c r="C63" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" t="s">
+        <v>54</v>
+      </c>
+      <c r="C64" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" t="s">
+        <v>55</v>
+      </c>
+      <c r="C65" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>51</v>
+      </c>
+      <c r="C66" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" t="s">
+        <v>47</v>
+      </c>
+      <c r="C67" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>7</v>
+      </c>
+      <c r="B68" t="s">
+        <v>51</v>
+      </c>
+      <c r="C68" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>56</v>
+      </c>
+      <c r="C69" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" t="s">
+        <v>57</v>
+      </c>
+      <c r="C70" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C71" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>